<commit_message>
Pyber with Pychart take 2 - 6-11-b
</commit_message>
<xml_diff>
--- a/Matplotlib/05-Matplotlib/Pyber/raw_data/city_data.xlsx
+++ b/Matplotlib/05-Matplotlib/Pyber/raw_data/city_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sivakumar\Desktop\Rutgers\python-challenge\Matplotlib\05-Matplotlib\Pyber\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{766501D4-5112-4DF9-98FC-E0D4E69F73BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71C06AC-664D-4C40-92E1-DCCFE84EFE2A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city_data" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1240,17 +1240,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C121"/>
+  <autoFilter ref="A1:C121" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>